<commit_message>
update log file with cuvette chamber conditions
</commit_message>
<xml_diff>
--- a/2023_field_campaign/licor_log_file_blank.xlsx
+++ b/2023_field_campaign/licor_log_file_blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/2023_field_campaign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F4AA34-0934-9748-8711-F63D6E5EB9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA802A4B-0AD5-D342-9B45-48CA659E6549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="500" windowWidth="48680" windowHeight="26540" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$H$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,37 +39,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">ID match user defined variable? </t>
-  </si>
-  <si>
-    <t>Tag ID</t>
-  </si>
-  <si>
-    <t>Species (Tri, Mai, Ari)</t>
-  </si>
-  <si>
-    <t>Performed auto match before curve?</t>
-  </si>
-  <si>
-    <t>Did leaf fit entire cuvette?</t>
-  </si>
-  <si>
-    <t>If not, was leaf area manually input through leaf width</t>
-  </si>
-  <si>
-    <t>Notes (e.g., issues with fitting leaf, whether a second curve was done, etc.)</t>
-  </si>
-  <si>
-    <t>Curve details (e.g., PAR; start time)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
+  <si>
+    <t>LICOR CHAMBER CONDITIONS</t>
+  </si>
+  <si>
+    <t>FLOW (μmol/s):</t>
+  </si>
+  <si>
+    <t>________________</t>
+  </si>
+  <si>
+    <t>VPDleaf (kPa):</t>
+  </si>
+  <si>
+    <t>CO2_r (μmol/mol):</t>
+  </si>
+  <si>
+    <t>FAN (rpm):</t>
+  </si>
+  <si>
+    <t>FLOW (degC):</t>
+  </si>
+  <si>
+    <t>Y / N</t>
+  </si>
+  <si>
+    <t>LIGHT (μmol/m^2/s):</t>
+  </si>
+  <si>
+    <t>*if other, explain in "notes section"</t>
+  </si>
+  <si>
+    <t>Q6. If "N" selected for Q5, was leaf area input through leaf width?*</t>
+  </si>
+  <si>
+    <t>Q5. Did leaf fit entire cuvette?*</t>
+  </si>
+  <si>
+    <t>Q4. Perform auto match before curve?*</t>
+  </si>
+  <si>
+    <t>Q3. ID matches user defined variable?*</t>
+  </si>
+  <si>
+    <t>Q2. Species (Tri, Mai, Ari)</t>
+  </si>
+  <si>
+    <t>Q1. Tag ID</t>
+  </si>
+  <si>
+    <t>Q7. Curve details (e.g., type of curve; start time)</t>
+  </si>
+  <si>
+    <t>Q8. Notes (e.g., issues with fitting leaf, whether a second curve was done,  etc.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,11 +109,31 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -129,6 +179,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,235 +503,456 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H20" sqref="A2:H20"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
+    <row r="1" spans="1:8" ht="162" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" ht="94" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:8" ht="94" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A26:E26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="52" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="50"/>
+  <pageSetup scale="48" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="50"/>
   <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;LDate: __________________&amp;CMachine (circle):
-Ozz   Gib    Alb    Stan    Yat&amp;RLicor Enthusiast: ____________________</oddHeader>
-    <oddFooter>&amp;LWeather notes:</oddFooter>
+    <oddHeader>&amp;L&amp;"Calibri (Body),Regular"&amp;24
+Date: __________________&amp;C&amp;"Calibri (Body),Regular"&amp;18Machine (circle):
+&amp;24Ozz   Gib    Alb    Stan    Yat&amp;R&amp;"Calibri (Body),Regular"&amp;20
+Licor Enthusiast: ____________________</oddHeader>
+    <oddFooter>&amp;L&amp;"Calibri (Body),Regular"&amp;20Weather notes:</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>